<commit_message>
Move bus speed factors from hardcoded to additional_inputs.xlsx
The speed factors that convert Google Maps car speeds to bus speeds are now
configurable in additional_inputs.xlsx (Buskosten sheet):

  snelheidsfactor_touringcar: 0.95
  snelheidsfactor_dubbeldekker: 0.90
  snelheidsfactor_lagevloer: 0.85
  snelheidsfactor_midibus: 0.92
  snelheidsfactor_taxibus: 0.95

Added load_bus_speed_factors() function to read these from Excel. This ensures
all assumptions are visible and configurable in the Excel file rather than
buried in Python code.

https://claude.ai/code/session_012BGwrrJFcdhXfAhz9aabQW
</commit_message>
<xml_diff>
--- a/additional_inputs.xlsx
+++ b/additional_inputs.xlsx
@@ -1039,7 +1039,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1955,6 +1955,66 @@
         <is>
           <t>km/h</t>
         </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Snelheidsfactor bus t.o.v. auto (Google Maps geeft autosnelheid):</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>snelheidsfactor_touringcar</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>snelheidsfactor_dubbeldekker</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>snelheidsfactor_lagevloer</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>snelheidsfactor_midibus</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>snelheidsfactor_taxibus</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update input data: fuel prices, matrices, tanklocaties (2026-02-06)
</commit_message>
<xml_diff>
--- a/additional_inputs.xlsx
+++ b/additional_inputs.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tarieven" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Chauffeurkosten" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Buskosten" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Duurzaamheid" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Brandstofprijzen" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarieven" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Chauffeurkosten" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Buskosten" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Duurzaamheid" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Brandstofprijzen" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -38,9 +38,6 @@
       <b val="1"/>
       <color rgb="002F5496"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -93,7 +90,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
@@ -103,7 +100,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -626,7 +622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1029,334 +1025,6 @@
       <c r="D21" s="4" t="inlineStr">
         <is>
           <t>Werkgeverslasten factor</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="inlineStr">
-        <is>
-          <t>ORT (Onregelmatigheidstoeslag) - Article 11 OV</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>ORT_weekday_start_hour</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>19</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>uur</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>ORT begint doordeweeks (19:00)</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>ORT_weekday_end_hour</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>uur</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>ORT eindigt doordeweeks (07:30)</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>ORT_weekday_rate_eur_per_hour</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>EUR/uur</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>ORT toeslag doordeweeks avond/nacht</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>ORT_saturday_rate_eur_per_hour</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>EUR/uur</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>ORT toeslag zaterdag (hele dag)</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>ORT_sunday_rate_eur_per_hour</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>6.68</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>EUR/uur</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>ORT toeslag zondag/feestdag (hele dag)</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="7" t="inlineStr">
-        <is>
-          <t>Overwerk toeslagen</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>overwerk_threshold_uren_per_maand</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>173.33</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>uren</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Drempel voor overwerk (173.33h/maand)</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>overwerk_toeslag_rijdend_pct</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>35</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Overwerktoeslag rijdend personeel</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>overwerk_toeslag_niet_rijdend_min_pct</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>30</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Overwerktoeslag niet-rijdend (min)</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>overwerk_toeslag_niet_rijdend_max_pct</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>100</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Overwerktoeslag niet-rijdend (max)</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="7" t="inlineStr">
-        <is>
-          <t>Maaltijdvergoedingen</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>maaltijd_threshold_1_uren</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>11</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>uren</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Dienst &gt;= 11 uur</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>maaltijd_vergoeding_1_eur</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Maaltijdvergoeding bij &gt;= 11 uur</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>maaltijd_threshold_2_uren</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>14</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>uren</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Dienst &gt;= 14 uur</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>maaltijd_vergoeding_2_eur</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>36.72</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Maaltijdvergoeding bij &gt;= 14 uur</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="7" t="inlineStr">
-        <is>
-          <t>Gebroken dienst toeslag</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>gebroken_dienst_min_onderbreking_min</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>120</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>minuten</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Minimale onderbreking voor gebroken dienst (2h)</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>gebroken_dienst_toeslag_eur</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>15</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Toeslag per gebroken dienst</t>
         </is>
       </c>
     </row>
@@ -2289,7 +1957,6 @@
         </is>
       </c>
     </row>
-    <row r="53"/>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
@@ -2545,7 +2212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2597,7 +2264,9 @@
           <t>diesel_b7_pompprijs_eur_per_liter</t>
         </is>
       </c>
-      <c r="B3" s="6" t="n"/>
+      <c r="B3" s="6" t="n">
+        <v>2.013</v>
+      </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
           <t>EUR/liter</t>
@@ -2606,6 +2275,11 @@
       <c r="D3" s="4" t="inlineStr">
         <is>
           <t>Diesel B7 pompprijs</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2026-02-06 17:01 (CBS: 2026MM01)</t>
         </is>
       </c>
     </row>
@@ -2663,6 +2337,7 @@
         </is>
       </c>
     </row>
+    <row r="7"/>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Increase max_extra_buses_pct from 30% to 50%
- Changed default exploration range to 50% more buses
- Made max_extra_buses_pct configurable via additional_inputs.xlsx
- Added to FinancialConfig and load_financial_config()
- Fixed default garage values in loader (60 min, 50 km)

This allows the profit optimizer to explore a wider range of bus counts
to find the true profit optimum.

https://claude.ai/code/session_012BGwrrJFcdhXfAhz9aabQW
</commit_message>
<xml_diff>
--- a/additional_inputs.xlsx
+++ b/additional_inputs.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarieven" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Chauffeurkosten" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Buskosten" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Duurzaamheid" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Brandstofprijzen" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Tarieven" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Chauffeurkosten" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Buskosten" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Duurzaamheid" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Brandstofprijzen" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -622,7 +622,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1026,6 +1026,28 @@
         <is>
           <t>Werkgeverslasten factor</t>
         </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Versie 8 optimalisatie:</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>max_extra_buses_pct</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2337,7 +2359,6 @@
         </is>
       </c>
     </row>
-    <row r="7"/>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>

</xml_diff>